<commit_message>
Added more test cases and data for vlink smoke test Debit.
</commit_message>
<xml_diff>
--- a/KatalonData/VLinkSmokeDataACH.xlsx
+++ b/KatalonData/VLinkSmokeDataACH.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5726F34A-48E4-4ECB-B9A1-AD63C784B306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{090AC336-65AB-429A-B057-3698832A4CFF}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="5" activeTab="5" xr2:uid="{388D034C-6DAD-459D-91DB-B99E6D26AB62}"/>
+    <workbookView activeTab="10" firstSheet="3" windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{388D034C-6DAD-459D-91DB-B99E6D26AB62}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Debit" sheetId="1" r:id="rId1"/>
-    <sheet name="Debit-ZeroDollar" sheetId="2" r:id="rId2"/>
-    <sheet name="Debit-Void" sheetId="3" r:id="rId3"/>
-    <sheet name="Debit-Credit" sheetId="4" r:id="rId4"/>
-    <sheet name="Debit-Credit-Void" sheetId="5" r:id="rId5"/>
-    <sheet name="Debit-MRF" sheetId="6" r:id="rId6"/>
+    <sheet name="Debit" r:id="rId1" sheetId="1"/>
+    <sheet name="Debit-ZeroDollar" r:id="rId2" sheetId="2"/>
+    <sheet name="Debit-Void" r:id="rId3" sheetId="3"/>
+    <sheet name="Debit-Credit" r:id="rId4" sheetId="4"/>
+    <sheet name="Debit-Credit-Void" r:id="rId5" sheetId="5"/>
+    <sheet name="Debit-MRF" r:id="rId6" sheetId="6"/>
+    <sheet name="Void-MRF" r:id="rId7" sheetId="7"/>
+    <sheet name="Credit-MRF" r:id="rId8" sheetId="8"/>
+    <sheet name="Debit-RemID-Pipe" r:id="rId9" sheetId="9"/>
+    <sheet name="DebitVoid-RemID-Pipe" r:id="rId10" sheetId="10"/>
+    <sheet name="DebitCredit-RemID-Pipe" r:id="rId11" sheetId="11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -41,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="296">
   <si>
     <t>Result</t>
   </si>
@@ -316,9 +321,6 @@
     <t>22201</t>
   </si>
   <si>
-    <t>Missing parameter: transaction_type</t>
-  </si>
-  <si>
     <t>Missing parameter: message_version</t>
   </si>
   <si>
@@ -328,52 +330,617 @@
     <t>Signon authentication error</t>
   </si>
   <si>
-    <t>Missing parameter: Response format</t>
-  </si>
-  <si>
-    <t>Missing parameter: check_type</t>
-  </si>
-  <si>
-    <t>Missing parameter: first name</t>
-  </si>
-  <si>
-    <t>Missing parameter: last name</t>
-  </si>
-  <si>
-    <t>Missing parameter: Address</t>
-  </si>
-  <si>
-    <t>Missing parameter: City</t>
-  </si>
-  <si>
-    <t>Missing parameter: state</t>
-  </si>
-  <si>
-    <t>Missing parameter: ZIP</t>
-  </si>
-  <si>
-    <t>Missing parameter:account_number</t>
-  </si>
-  <si>
-    <t>Missing parameter: account_type</t>
-  </si>
-  <si>
-    <t>Missing parameter: rtn</t>
-  </si>
-  <si>
-    <t>Missing parameter: amount</t>
-  </si>
-  <si>
-    <t>Missing parameter: sec</t>
-  </si>
-  <si>
-    <t>Missing parameter: compane_name</t>
+    <t>Invalid transaction type</t>
+  </si>
+  <si>
+    <t>response_format</t>
+  </si>
+  <si>
+    <t>Bank Account type not valid</t>
+  </si>
+  <si>
+    <t>check_first_name</t>
+  </si>
+  <si>
+    <t>check_last_name</t>
+  </si>
+  <si>
+    <t>check_zip</t>
+  </si>
+  <si>
+    <t>check_state</t>
+  </si>
+  <si>
+    <t>check_city</t>
+  </si>
+  <si>
+    <t>check_address</t>
+  </si>
+  <si>
+    <t>check_company, check_company</t>
+  </si>
+  <si>
+    <t>standard_entry_class</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>routing_number</t>
+  </si>
+  <si>
+    <t>account_type</t>
+  </si>
+  <si>
+    <t>check_account</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:49:44 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:50:10 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:50:34 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:50:56 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:51:19 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:51:42 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:52:05 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:52:26 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:52:48 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:53:09 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:53:31 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:53:54 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:54:15 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:54:38 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:54:59 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:55:21 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:55:43 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:56:05 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 13:56:26 EST 2023</t>
+  </si>
+  <si>
+    <t>TranxID</t>
+  </si>
+  <si>
+    <t>OriginalTranType</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:16:28 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:16:43 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:16:55 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:17:05 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:17:16 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:17:27 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:17:38 EST 2023</t>
+  </si>
+  <si>
+    <t>check_first_name, check_last_name, check_address, check_city, check_state, che</t>
+  </si>
+  <si>
+    <t>12124566</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:25:18 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:25:32 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:25:43 EST 2023</t>
+  </si>
+  <si>
+    <t>12345678</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:56:13 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:56:29 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:56:42 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:56:55 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:57:07 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:57:32 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:57:44 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:58:09 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:58:21 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 16:58:33 EST 2023</t>
+  </si>
+  <si>
+    <t>response_format, check_first_name, check_last_name, check_address, check_city</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:01:35 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:01:50 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:15:50 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:16:10 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:16:28 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:16:46 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:17:04 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:17:21 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:17:39 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:26:31 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:27:04 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:27:33 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:28:04 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:28:32 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:29:02 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:29:32 EST 2023</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:36:29 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:37:02 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:37:34 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:38:05 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:38:35 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:39:07 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:39:38 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:44:56 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:45:17 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:45:36 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:45:54 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:46:12 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:46:30 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:46:49 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:47:08 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:47:25 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:47:43 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:48:01 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:48:18 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:48:36 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:48:55 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:49:13 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:49:42 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:50:11 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:50:41 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:51:10 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:51:40 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:52:10 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:52:42 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:53:13 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:53:44 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:54:15 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:54:46 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:55:17 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:55:49 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:56:21 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:57:03 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:57:45 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:58:26 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:59:08 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 17:59:52 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:00:35 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:01:19 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:01:51 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:02:22 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:02:52 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:03:23 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:03:55 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:04:27 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:04:58 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:05:16 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:05:34 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:05:51 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:06:09 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:06:27 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:06:45 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:07:04 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:07:33 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:08:02 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:08:32 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:09:02 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:09:31 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 18:10:01 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:16:32 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:16:52 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:17:11 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:17:30 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:17:49 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:18:07 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:18:25 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:18:43 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:19:01 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:19:18 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:19:35 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:19:53 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:20:11 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:20:29 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:20:47 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:21:16 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:21:46 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:22:15 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:22:45 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:23:14 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:23:44 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:24:13 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:24:44 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:25:16 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:26:04 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:26:35 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:27:06 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:27:38 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:28:19 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:29:01 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:29:45 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:30:27 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:31:10 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:31:54 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:32:36 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:33:07 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:33:38 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:34:10 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:34:41 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:35:11 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:35:43 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:36:14 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:36:32 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:36:50 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:37:08 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:37:26 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:37:44 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:38:02 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:38:21 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:38:50 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:39:19 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:39:50 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:40:19 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:40:48 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 19:41:16 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 20:06:22 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 20:06:55 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 20:07:27 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 20:07:58 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 20:08:29 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 20:09:00 EST 2023</t>
+  </si>
+  <si>
+    <t>Thu Jan 19 20:09:32 EST 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,23 +989,23 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -455,10 +1022,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -493,7 +1060,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -545,7 +1112,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -656,21 +1223,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -687,7 +1254,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -739,15 +1306,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme 2013 - 2022" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F1F3D5-37B4-4D18-A029-08788223EDF8}">
-  <dimension ref="A1:Q8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6F1F3D5-37B4-4D18-A029-08788223EDF8}">
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -755,20 +1322,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="3" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.5703125" style="3" collapsed="1"/>
-    <col min="8" max="8" width="11.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="12.5703125" style="3" collapsed="1"/>
+    <col min="1" max="1" style="3" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" style="3" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" style="3" width="12.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="11.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="3" width="15.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="3" width="14.85546875" collapsed="true"/>
+    <col min="11" max="16384" style="3" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="21.75" r="1" s="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -826,7 +1393,7 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>234</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>17</v>
@@ -873,7 +1440,7 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>235</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>17</v>
@@ -920,7 +1487,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>236</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>17</v>
@@ -967,7 +1534,7 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>237</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>17</v>
@@ -1014,7 +1581,7 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>238</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -1061,7 +1628,7 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>239</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>17</v>
@@ -1108,7 +1675,7 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>240</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>17</v>
@@ -1151,17 +1718,837 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{483E6572-E2E1-46C7-90FD-43A4857206DE}">
+  <dimension ref="A1:R8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" style="3" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" style="3" width="12.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="11.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="3" width="15.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="3" width="14.85546875" collapsed="true"/>
+    <col min="11" max="16384" style="3" width="12.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" customHeight="1" ht="21.75" r="1" s="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>282</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2">
+        <v>234</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2">
+        <v>234</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2">
+        <v>234</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>285</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2">
+        <v>234</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2">
+        <v>234</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>287</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2">
+        <v>234</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2">
+        <v>234</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DEB1C2-0C49-4D7C-B8E8-62617B390DA3}">
+  <dimension ref="A1:R8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" style="3" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" style="3" width="12.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="11.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="3" width="15.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="3" width="14.85546875" collapsed="true"/>
+    <col min="11" max="16384" style="3" width="12.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" customHeight="1" ht="21.75" r="1" s="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2">
+        <v>234</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>269</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2">
+        <v>234</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2">
+        <v>234</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2">
+        <v>234</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>272</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2">
+        <v>234</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>273</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2">
+        <v>234</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>274</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2">
+        <v>234</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F77AD1-6B6A-4837-8643-295057715D44}">
-  <dimension ref="A1:Q8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F77AD1-6B6A-4837-8643-295057715D44}">
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4:D8"/>
@@ -1169,20 +2556,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="3" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.5703125" style="3" collapsed="1"/>
-    <col min="8" max="8" width="11.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="12.5703125" style="3" collapsed="1"/>
+    <col min="1" max="1" style="3" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" style="3" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" style="3" width="12.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="11.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="3" width="15.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="3" width="14.85546875" collapsed="true"/>
+    <col min="11" max="16384" style="3" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="21.75" r="1" s="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +2627,7 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>241</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>17</v>
@@ -1287,7 +2674,7 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>242</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>17</v>
@@ -1334,7 +2721,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>243</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>17</v>
@@ -1381,7 +2768,7 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>244</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>17</v>
@@ -1428,7 +2815,7 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>245</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -1475,7 +2862,7 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>246</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>17</v>
@@ -1522,7 +2909,7 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>247</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>17</v>
@@ -1565,13 +2952,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E9B566-2104-4D91-9419-2327ED3CE217}">
-  <dimension ref="A1:Q8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E9B566-2104-4D91-9419-2327ED3CE217}">
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -1579,20 +2966,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="3" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.5703125" style="3" collapsed="1"/>
-    <col min="8" max="8" width="11.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="12.5703125" style="3" collapsed="1"/>
+    <col min="1" max="1" style="3" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" style="3" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" style="3" width="12.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="11.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="3" width="15.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="3" width="14.85546875" collapsed="true"/>
+    <col min="11" max="16384" style="3" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="21.75" r="1" s="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1650,7 +3037,7 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>248</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>17</v>
@@ -1697,7 +3084,7 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>249</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>17</v>
@@ -1744,7 +3131,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>17</v>
@@ -1791,7 +3178,7 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>251</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>17</v>
@@ -1838,7 +3225,7 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>252</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -1885,7 +3272,7 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>253</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>17</v>
@@ -1932,7 +3319,7 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>254</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>17</v>
@@ -1975,13 +3362,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4157F26B-1901-489C-8F43-B30441C51CC9}">
-  <dimension ref="A1:Q8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4157F26B-1901-489C-8F43-B30441C51CC9}">
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -1989,20 +3376,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="3" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.5703125" style="3" collapsed="1"/>
-    <col min="8" max="8" width="11.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="12.5703125" style="3" collapsed="1"/>
+    <col min="1" max="1" style="3" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" style="3" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" style="3" width="12.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="11.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="3" width="15.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="3" width="14.85546875" collapsed="true"/>
+    <col min="11" max="16384" style="3" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="21.75" r="1" s="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2060,7 +3447,7 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>289</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>17</v>
@@ -2107,7 +3494,7 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>290</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>17</v>
@@ -2154,7 +3541,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>291</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>17</v>
@@ -2201,7 +3588,7 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>292</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>17</v>
@@ -2248,7 +3635,7 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>293</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -2295,7 +3682,7 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>294</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>17</v>
@@ -2342,7 +3729,7 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>295</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>17</v>
@@ -2385,13 +3772,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF09B7C8-12B8-4591-9AA2-4B82A69A8ABA}">
-  <dimension ref="A1:Q8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF09B7C8-12B8-4591-9AA2-4B82A69A8ABA}">
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -2399,20 +3786,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="3" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" style="3" collapsed="1"/>
-    <col min="6" max="6" width="13.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.5703125" style="3" collapsed="1"/>
-    <col min="8" max="8" width="11.7109375" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="12.5703125" style="3" collapsed="1"/>
+    <col min="1" max="1" style="3" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" style="3" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" style="3" width="12.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="11.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="3" width="15.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="3" width="14.85546875" collapsed="true"/>
+    <col min="11" max="16384" style="3" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="21.75" r="1" s="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2470,7 +3857,7 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>261</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>17</v>
@@ -2517,7 +3904,7 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>262</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>17</v>
@@ -2564,7 +3951,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>263</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>17</v>
@@ -2611,7 +3998,7 @@
         <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>264</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>17</v>
@@ -2658,7 +4045,7 @@
         <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>265</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
@@ -2705,7 +4092,7 @@
         <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>266</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>17</v>
@@ -2752,7 +4139,7 @@
         <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>267</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>17</v>
@@ -2795,40 +4182,34 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA08836-3194-499F-99DE-E912B383D439}">
-  <dimension ref="A1:AC20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA08836-3194-499F-99DE-E912B383D439}">
+  <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="3" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.28515625" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.140625" style="3" customWidth="1"/>
-    <col min="6" max="7" width="9.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="3" collapsed="1"/>
-    <col min="9" max="9" width="13.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.5703125" style="3" collapsed="1"/>
-    <col min="11" max="11" width="12.5703125" style="3"/>
-    <col min="12" max="12" width="12.5703125" style="3" collapsed="1"/>
-    <col min="13" max="14" width="12.5703125" style="3"/>
-    <col min="15" max="15" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="12.5703125" style="3"/>
-    <col min="19" max="24" width="12.5703125" style="3" collapsed="1"/>
-    <col min="25" max="29" width="12.5703125" style="3"/>
-    <col min="30" max="16384" width="12.5703125" style="3" collapsed="1"/>
+    <col min="1" max="1" style="3" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="36.140625" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="8" max="8" style="3" width="12.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
+    <col min="10" max="14" style="3" width="12.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="3" width="14.85546875" collapsed="true"/>
+    <col min="16" max="16384" style="3" width="12.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="21.75" r="1" s="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2903,13 +4284,17 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
       <c r="D2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>83</v>
@@ -2964,13 +4349,17 @@
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
       <c r="D3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>82</v>
@@ -3025,13 +4414,17 @@
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>82</v>
@@ -3087,13 +4480,17 @@
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
       <c r="D5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>82</v>
@@ -3149,13 +4546,17 @@
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>82</v>
@@ -3211,8 +4612,12 @@
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7"/>
-      <c r="B7"/>
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>114</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>17</v>
       </c>
@@ -3273,8 +4678,12 @@
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8"/>
-      <c r="B8"/>
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>17</v>
       </c>
@@ -3334,8 +4743,12 @@
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9"/>
-      <c r="B9"/>
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>116</v>
+      </c>
       <c r="D9" s="3" t="s">
         <v>17</v>
       </c>
@@ -3395,8 +4808,12 @@
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10"/>
-      <c r="B10"/>
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>117</v>
+      </c>
       <c r="D10" s="3" t="s">
         <v>17</v>
       </c>
@@ -3456,13 +4873,17 @@
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11"/>
-      <c r="B11"/>
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
       <c r="D11" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>82</v>
@@ -3517,13 +4938,17 @@
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12"/>
-      <c r="B12"/>
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
+      </c>
       <c r="D12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>82</v>
@@ -3578,13 +5003,17 @@
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13"/>
-      <c r="B13"/>
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>120</v>
+      </c>
       <c r="D13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>82</v>
@@ -3639,13 +5068,17 @@
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14"/>
-      <c r="B14"/>
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
       <c r="D14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>82</v>
@@ -3700,13 +5133,17 @@
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15"/>
-      <c r="B15"/>
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
       <c r="D15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>82</v>
@@ -3761,13 +5198,17 @@
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A16"/>
-      <c r="B16"/>
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>123</v>
+      </c>
       <c r="D16" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>82</v>
@@ -3822,13 +5263,17 @@
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A17"/>
-      <c r="B17"/>
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>124</v>
+      </c>
       <c r="D17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>82</v>
@@ -3883,13 +5328,17 @@
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18"/>
-      <c r="B18"/>
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>125</v>
+      </c>
       <c r="D18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>82</v>
@@ -3944,13 +5393,17 @@
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19"/>
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>126</v>
+      </c>
       <c r="D19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>82</v>
@@ -4005,13 +5458,17 @@
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20"/>
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>127</v>
+      </c>
       <c r="D20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>82</v>
@@ -4067,6 +5524,1556 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06482146-3F5D-47DF-9B90-B5700E0EE57E}">
+  <dimension ref="A1:P11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="36.140625" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="8" max="8" style="3" width="12.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
+    <col min="10" max="14" style="3" width="12.5703125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="3" width="19.7109375" collapsed="true"/>
+    <col min="16" max="16384" style="3" width="12.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" customHeight="1" ht="21.75" r="1" s="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="2">
+        <v>234</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="2">
+        <v>234</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="2">
+        <v>234</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="2">
+        <v>234</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="2">
+        <v>234</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="2">
+        <v>234</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="2">
+        <v>234</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="2">
+        <v>234</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="2">
+        <v>234</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F6E92C-F0B2-419E-A8FB-B67C2DE09DC4}">
+  <dimension ref="A1:R13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="36.140625" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="8" max="8" style="3" width="12.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
+    <col min="10" max="15" style="3" width="12.5703125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="3" width="15.42578125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="3" width="15.0" collapsed="true"/>
+    <col min="18" max="16384" style="3" width="12.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" customHeight="1" ht="21.75" r="1" s="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="2">
+        <v>234</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="2">
+        <v>234</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="2">
+        <v>234</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="2">
+        <v>234</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="2">
+        <v>234</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="2">
+        <v>234</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="2">
+        <v>234</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>155</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="2">
+        <v>234</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="2">
+        <v>234</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="2">
+        <v>234</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
+        <v>152</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="2">
+        <v>234</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475D3EEC-13EC-491F-9A96-22DFFF4616CF}">
+  <dimension ref="A1:R8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="3" width="25.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="18.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="3" width="9.7109375" collapsed="true"/>
+    <col min="5" max="5" style="3" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="3" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" style="3" width="12.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="3" width="11.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="3" width="15.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="3" width="14.85546875" collapsed="true"/>
+    <col min="11" max="16384" style="3" width="12.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row customFormat="1" customHeight="1" ht="21.75" r="1" s="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2">
+        <v>234</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2">
+        <v>234</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2">
+        <v>234</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="2">
+        <v>234</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2">
+        <v>234</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2">
+        <v>234</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2">
+        <v>234</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1773</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>